<commit_message>
update GLUE benchmark results
</commit_message>
<xml_diff>
--- a/LLM-adaptations-comparison.xlsx
+++ b/LLM-adaptations-comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom-b\Documents\Dossier centrale\Projets github\PrivateTinyBertGlue\PrivateTinyBertGlue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1691083E-E75D-43F6-82A1-07171DAE3D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFDFFBD-11E3-478D-AA30-4E4E78593A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-370" windowWidth="19420" windowHeight="11020" xr2:uid="{CC44CC4B-98D3-A24D-BA53-6CC7B6690794}"/>
+    <workbookView xWindow="5970" yWindow="1710" windowWidth="16695" windowHeight="10155" xr2:uid="{CC44CC4B-98D3-A24D-BA53-6CC7B6690794}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Dataset</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>epsilon = 4</t>
+  </si>
+  <si>
+    <t>256-384</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <dimension ref="B3:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -473,10 +476,18 @@
       <c r="C5" s="1">
         <v>1538</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="D5" s="1">
+        <v>5378</v>
+      </c>
+      <c r="E5" s="1">
+        <v>8450</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4391556</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -556,11 +567,21 @@
       <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="C14" s="1">
+        <v>1538</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5378</v>
+      </c>
+      <c r="E14" s="1">
+        <v>8450</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4391556</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -594,9 +615,15 @@
       <c r="B17" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="C17" s="1">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1">
+        <v>75</v>
+      </c>
+      <c r="E17" s="1">
+        <v>79.400000000000006</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>

</xml_diff>

<commit_message>
change max_len padding for qnli
</commit_message>
<xml_diff>
--- a/LLM-adaptations-comparison.xlsx
+++ b/LLM-adaptations-comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom-b\Documents\Dossier centrale\Projets github\PrivateTinyBertGlue\PrivateTinyBertGlue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A64EA1-368F-4D51-AB1E-DAA40D15AB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C0577A-2CE4-4800-8E39-BCBE058B46D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5970" yWindow="1710" windowWidth="16695" windowHeight="10155" xr2:uid="{CC44CC4B-98D3-A24D-BA53-6CC7B6690794}"/>
+    <workbookView xWindow="6150" yWindow="945" windowWidth="16695" windowHeight="10155" xr2:uid="{CC44CC4B-98D3-A24D-BA53-6CC7B6690794}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42DAD82-B324-D54C-AFE5-D35C7A0D2F76}">
   <dimension ref="B3:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -502,7 +502,9 @@
       <c r="E6" s="1">
         <v>75.099999999999994</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>78.599999999999994</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>